<commit_message>
Updated Flynn Dam Heights
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DateTime</t>
   </si>
@@ -50,7 +50,10 @@
     <t>Heavy rain the day before (~0.58-0.75" according to CoCoRaHS)</t>
   </si>
   <si>
-    <t>Rained this morning (~023" according to CoCoRaHS)</t>
+    <t>Brush may have been removed from grate</t>
+  </si>
+  <si>
+    <t>Rained this morning (~0.23" according to CoCoRaHS)</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -472,7 +475,7 @@
         <v>2.29</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -481,6 +484,17 @@
       </c>
       <c r="B13">
         <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45058.433333333334</v>
+      </c>
+      <c r="B14">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Flynn Dam Data
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>DateTime</t>
   </si>
@@ -53,10 +54,22 @@
     <t>Brush may have been removed from grate</t>
   </si>
   <si>
-    <t>Rained this morning (~0.23" according to CoCoRaHS)</t>
-  </si>
-  <si>
     <t>Was windy/wavy so could have been 2.09</t>
+  </si>
+  <si>
+    <t>Rain over night (~0.21-0.27" according to CoCoRaHS)</t>
+  </si>
+  <si>
+    <t>Rain this morning (~0.23" according to CoCoRaHS)</t>
+  </si>
+  <si>
+    <t>Slight rain in morning before measurement (~0.02" according to CoCoRaHS)</t>
+  </si>
+  <si>
+    <t>No rain</t>
+  </si>
+  <si>
+    <t>Rain</t>
   </si>
 </sst>
 </file>
@@ -375,23 +388,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -399,32 +415,38 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45048.45208333333</v>
       </c>
       <c r="B5">
         <v>2.34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>0.66</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45050.508333333331</v>
       </c>
       <c r="B6">
         <v>2.3199999999999998</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45051.636111111111</v>
       </c>
@@ -432,7 +454,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45052.484722222223</v>
       </c>
@@ -440,18 +462,21 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45053.447916666664</v>
       </c>
       <c r="B9">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45054.690972222219</v>
       </c>
@@ -459,29 +484,35 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45055.57708333333</v>
       </c>
       <c r="B11">
         <v>2.29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45056.46597222222</v>
       </c>
       <c r="B12">
         <v>2.29</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0.25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45057.388194444444</v>
       </c>
@@ -489,18 +520,18 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45058.433333333334</v>
       </c>
       <c r="B14">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45059.370833333334</v>
       </c>
@@ -508,7 +539,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45060.85833333333</v>
       </c>
@@ -516,7 +547,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45061.70208333333</v>
       </c>
@@ -524,7 +555,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45062.5</v>
       </c>
@@ -532,7 +563,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45063.567361111112</v>
       </c>
@@ -540,15 +571,134 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45064.477083333331</v>
       </c>
       <c r="B20">
         <v>2.1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45065.518750000003</v>
+      </c>
+      <c r="B21">
+        <v>2.13</v>
+      </c>
+      <c r="C21">
+        <v>0.25</v>
+      </c>
+      <c r="D21" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45066.513194444444</v>
+      </c>
+      <c r="B22">
+        <v>2.1</v>
+      </c>
+      <c r="C22">
+        <v>0.02</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45067.513888888891</v>
+      </c>
+      <c r="B23">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45068.533333333333</v>
+      </c>
+      <c r="B24">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45069.490277777775</v>
+      </c>
+      <c r="B25">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45070.518750000003</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>45071.504861111112</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45072.555555555555</v>
+      </c>
+      <c r="B28">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>45073.413888888892</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45073.726388888892</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45074.857638888891</v>
+      </c>
+      <c r="B31">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>45075.468055555553</v>
+      </c>
+      <c r="B32">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45076.54583333333</v>
+      </c>
+      <c r="B33">
+        <v>1.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some old hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>DateTime</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Water upstream of dam completely iced over</t>
+  </si>
+  <si>
+    <t>Ice on gauge, difficult to read</t>
   </si>
 </sst>
 </file>
@@ -496,12 +499,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D263"/>
+  <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
+      <selection pane="bottomLeft" activeCell="C267" sqref="C267:D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3168,6 +3171,53 @@
         <v>50</v>
       </c>
     </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A264" s="1">
+        <v>45307.541666666664</v>
+      </c>
+      <c r="B264" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="D264" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A265" s="1">
+        <v>45308.479166666664</v>
+      </c>
+      <c r="B265" s="2">
+        <v>1.91</v>
+      </c>
+      <c r="C265">
+        <v>0.02</v>
+      </c>
+      <c r="D265" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A266" s="1">
+        <v>45309.510416666664</v>
+      </c>
+      <c r="B266" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A267" s="1">
+        <v>45310.510416666664</v>
+      </c>
+      <c r="B267" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="C267">
+        <v>0.02</v>
+      </c>
+      <c r="D267" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Start of GC trails
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -511,12 +511,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D297"/>
+  <dimension ref="A1:D298"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D290" sqref="D290:D297"/>
+      <selection pane="bottomLeft" activeCell="C298" sqref="C298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,6 +3512,14 @@
         <v>55</v>
       </c>
     </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A298" s="1">
+        <v>45341.588194444441</v>
+      </c>
+      <c r="B298" s="2">
+        <v>1.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more Superstition Trails
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -511,12 +511,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D298"/>
+  <dimension ref="A1:D299"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C298" sqref="C298"/>
+      <selection pane="bottomLeft" activeCell="C299" sqref="C299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3520,6 +3520,14 @@
         <v>1.85</v>
       </c>
     </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A299" s="1">
+        <v>45342.565972222219</v>
+      </c>
+      <c r="B299" s="2">
+        <v>1.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Work on deadend breaks
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -511,12 +511,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D306"/>
+  <dimension ref="A1:D308"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C306" sqref="C306"/>
+      <selection pane="bottomLeft" activeCell="A309" sqref="A309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3584,6 +3584,22 @@
         <v>1.84</v>
       </c>
     </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" s="1">
+        <v>45350.493055555555</v>
+      </c>
+      <c r="B307" s="2">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" s="1">
+        <v>45351.424305555556</v>
+      </c>
+      <c r="B308" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Weekly update, incl Eagle Lake ice out
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
   <si>
     <t>DateTime</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>actual rain, not SWE</t>
+  </si>
+  <si>
+    <t>Flynn lake ice out</t>
+  </si>
+  <si>
+    <t>Eagle lake ice out</t>
   </si>
 </sst>
 </file>
@@ -514,12 +520,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D317"/>
+  <dimension ref="A1:D324"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A300" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C317" sqref="C317"/>
+      <selection pane="bottomLeft" activeCell="C324" sqref="C324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3681,6 +3687,68 @@
         <v>1.83</v>
       </c>
     </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A318" s="1">
+        <v>45361.55</v>
+      </c>
+      <c r="B318" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A319" s="1">
+        <v>45362.652777777781</v>
+      </c>
+      <c r="B319" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D319" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A320" s="1">
+        <v>45363.5</v>
+      </c>
+      <c r="B320" s="2">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A321" s="1">
+        <v>45364.668055555558</v>
+      </c>
+      <c r="B321" s="2">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A322" s="1">
+        <v>45365.63958333333</v>
+      </c>
+      <c r="B322" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D322" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A323" s="1">
+        <v>45366.557638888888</v>
+      </c>
+      <c r="B323" s="2">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A324" s="1">
+        <v>45367.664583333331</v>
+      </c>
+      <c r="B324" s="2">
+        <v>1.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Eagle ice-out post
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -520,12 +520,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D324"/>
+  <dimension ref="A1:D325"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A300" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C324" sqref="C324"/>
+      <selection pane="bottomLeft" activeCell="B326" sqref="B326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3749,6 +3749,14 @@
         <v>1.85</v>
       </c>
     </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A325" s="1">
+        <v>45368.538888888892</v>
+      </c>
+      <c r="B325" s="2">
+        <v>1.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added NC hikes (with updates to code in others)
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="74">
   <si>
     <t>DateTime</t>
   </si>
@@ -565,12 +565,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E429"/>
+  <dimension ref="A1:E436"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A429" sqref="A429"/>
+      <selection pane="bottomLeft" activeCell="D436" sqref="D436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6166,6 +6166,95 @@
         <v>2.11</v>
       </c>
     </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>62</v>
+      </c>
+      <c r="B430" s="1">
+        <v>45473.5625</v>
+      </c>
+      <c r="C430" s="2">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="D430">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>62</v>
+      </c>
+      <c r="B431" s="1">
+        <v>45474.693749999999</v>
+      </c>
+      <c r="C431" s="2">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>62</v>
+      </c>
+      <c r="B432" s="1">
+        <v>45475.651388888888</v>
+      </c>
+      <c r="C432" s="2">
+        <v>2</v>
+      </c>
+      <c r="D432">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>62</v>
+      </c>
+      <c r="B433" s="1">
+        <v>45476.453472222223</v>
+      </c>
+      <c r="C433" s="2">
+        <v>2</v>
+      </c>
+      <c r="D433">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>62</v>
+      </c>
+      <c r="B434" s="1">
+        <v>45477.530555555553</v>
+      </c>
+      <c r="C434" s="2">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>62</v>
+      </c>
+      <c r="B435" s="1">
+        <v>45478.490277777775</v>
+      </c>
+      <c r="C435" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="D435">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>62</v>
+      </c>
+      <c r="B436" s="1">
+        <v>45479.515972222223</v>
+      </c>
+      <c r="C436" s="2">
+        <v>1.96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Red Rocks Hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="88">
   <si>
     <t>DateTime</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Snowing at observation time</t>
+  </si>
+  <si>
+    <t>Cleaned grate before reading; some rain right before reading</t>
   </si>
 </sst>
 </file>
@@ -604,12 +607,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E555"/>
+  <dimension ref="A1:E557"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D555" sqref="D555"/>
+      <selection pane="bottomLeft" activeCell="E558" sqref="E558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7816,6 +7819,34 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>62</v>
+      </c>
+      <c r="B556" s="1">
+        <v>45599.45416666667</v>
+      </c>
+      <c r="C556" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A557" t="s">
+        <v>62</v>
+      </c>
+      <c r="B557" s="1">
+        <v>45600.450694444444</v>
+      </c>
+      <c r="C557" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="D557">
+        <v>0.52</v>
+      </c>
+      <c r="E557" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reorganized Other Notable Hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="88">
   <si>
     <t>DateTime</t>
   </si>
@@ -607,12 +607,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E557"/>
+  <dimension ref="A1:E558"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E558" sqref="E558"/>
+      <selection pane="bottomLeft" activeCell="D558" sqref="D558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7847,6 +7847,20 @@
         <v>87</v>
       </c>
     </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A558" t="s">
+        <v>62</v>
+      </c>
+      <c r="B558" s="1">
+        <v>45601.374305555553</v>
+      </c>
+      <c r="C558" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="D558">
+        <v>0.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added chur St Luzi
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="88">
   <si>
     <t>DateTime</t>
   </si>
@@ -607,12 +607,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E559"/>
+  <dimension ref="A1:E562"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A559" sqref="A559"/>
+      <selection pane="bottomLeft" activeCell="B562" sqref="B562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7875,6 +7875,39 @@
         <v>0.34</v>
       </c>
     </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A560" t="s">
+        <v>62</v>
+      </c>
+      <c r="B560" s="1">
+        <v>45603.520833333336</v>
+      </c>
+      <c r="C560" s="2">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A561" t="s">
+        <v>62</v>
+      </c>
+      <c r="B561" s="1">
+        <v>45604.463194444441</v>
+      </c>
+      <c r="C561" s="2">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A562" t="s">
+        <v>62</v>
+      </c>
+      <c r="B562" s="1">
+        <v>45605.49722222222</v>
+      </c>
+      <c r="C562" s="2">
+        <v>1.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Lauterbrunnen, Started edits to Iowa
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="96">
   <si>
     <t>DateTime</t>
   </si>
@@ -631,12 +631,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E586"/>
+  <dimension ref="A1:E589"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B587" sqref="B587"/>
+      <selection pane="bottomLeft" activeCell="E589" sqref="E589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8250,6 +8250,51 @@
         <v>1.89</v>
       </c>
     </row>
+    <row r="587" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A587" t="s">
+        <v>62</v>
+      </c>
+      <c r="B587" s="1">
+        <v>45630.5</v>
+      </c>
+      <c r="C587" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D587">
+        <v>0.1</v>
+      </c>
+      <c r="E587" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A588" t="s">
+        <v>62</v>
+      </c>
+      <c r="B588" s="1">
+        <v>45631.545138888891</v>
+      </c>
+      <c r="C588" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D588">
+        <v>0.1</v>
+      </c>
+      <c r="E588" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A589" t="s">
+        <v>62</v>
+      </c>
+      <c r="B589" s="1">
+        <v>45632.525000000001</v>
+      </c>
+      <c r="C589" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Musegg Wall walk
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="96">
   <si>
     <t>DateTime</t>
   </si>
@@ -631,12 +631,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E592"/>
+  <dimension ref="A1:E599"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C593" sqref="C593"/>
+      <selection pane="bottomLeft" activeCell="A599" sqref="A599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8334,6 +8334,104 @@
         <v>91</v>
       </c>
     </row>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A593" t="s">
+        <v>62</v>
+      </c>
+      <c r="B593" s="1">
+        <v>45636.502083333333</v>
+      </c>
+      <c r="C593" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D593">
+        <v>0.01</v>
+      </c>
+      <c r="E593" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="594" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A594" t="s">
+        <v>62</v>
+      </c>
+      <c r="B594" s="1">
+        <v>45637.479861111111</v>
+      </c>
+      <c r="C594" s="2">
+        <v>1.91</v>
+      </c>
+      <c r="D594">
+        <v>0.04</v>
+      </c>
+      <c r="E594" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A595" t="s">
+        <v>62</v>
+      </c>
+      <c r="B595" s="1">
+        <v>45638.552083333336</v>
+      </c>
+      <c r="C595" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D595">
+        <v>0.04</v>
+      </c>
+      <c r="E595" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="596" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A596" t="s">
+        <v>62</v>
+      </c>
+      <c r="B596" s="1">
+        <v>45639.5</v>
+      </c>
+      <c r="C596" s="2">
+        <v>1.89</v>
+      </c>
+      <c r="E596" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A597" t="s">
+        <v>62</v>
+      </c>
+      <c r="B597" s="1">
+        <v>45640.458333333336</v>
+      </c>
+      <c r="C597" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A598" t="s">
+        <v>62</v>
+      </c>
+      <c r="B598" s="1">
+        <v>45641.5</v>
+      </c>
+      <c r="C598" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A599" t="s">
+        <v>62</v>
+      </c>
+      <c r="B599" s="1">
+        <v>45642.427083333336</v>
+      </c>
+      <c r="C599" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Lucerne Bridges Walk
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="96">
   <si>
     <t>DateTime</t>
   </si>
@@ -631,12 +631,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E599"/>
+  <dimension ref="A1:E602"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A599" sqref="A599"/>
+      <selection pane="bottomLeft" activeCell="A602" sqref="A602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8432,6 +8432,51 @@
         <v>1.88</v>
       </c>
     </row>
+    <row r="600" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A600" t="s">
+        <v>62</v>
+      </c>
+      <c r="B600" s="1">
+        <v>45643.581944444442</v>
+      </c>
+      <c r="C600" s="2">
+        <v>1.88</v>
+      </c>
+      <c r="D600">
+        <v>0.01</v>
+      </c>
+      <c r="E600" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A601" t="s">
+        <v>62</v>
+      </c>
+      <c r="B601" s="1">
+        <v>45644.466666666667</v>
+      </c>
+      <c r="C601" s="2">
+        <v>1.88</v>
+      </c>
+      <c r="D601">
+        <v>0.01</v>
+      </c>
+      <c r="E601" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A602" t="s">
+        <v>62</v>
+      </c>
+      <c r="B602" s="1">
+        <v>45645.473611111112</v>
+      </c>
+      <c r="C602" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting to add MN hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="101">
   <si>
     <t>DateTime</t>
   </si>
@@ -646,12 +646,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E635"/>
+  <dimension ref="A1:E636"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A616" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A622" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E631" sqref="E631"/>
+      <selection pane="bottomLeft" activeCell="E636" sqref="E636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8924,6 +8924,23 @@
         <v>91</v>
       </c>
     </row>
+    <row r="636" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A636" t="s">
+        <v>62</v>
+      </c>
+      <c r="B636" s="1">
+        <v>45313.604166666664</v>
+      </c>
+      <c r="C636" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="D636">
+        <v>0.03</v>
+      </c>
+      <c r="E636" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Chester Creek and Gooseberry
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="101">
   <si>
     <t>DateTime</t>
   </si>
@@ -646,12 +646,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E640"/>
+  <dimension ref="A1:E642"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A622" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D640" sqref="D640"/>
+      <selection pane="bottomLeft" activeCell="A641" sqref="A641:A642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8985,6 +8985,31 @@
         <v>1.86</v>
       </c>
     </row>
+    <row r="641" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A641" t="s">
+        <v>62</v>
+      </c>
+      <c r="B641" s="1">
+        <v>45684.5</v>
+      </c>
+      <c r="C641" s="2">
+        <v>1.86</v>
+      </c>
+      <c r="E641" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="642" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A642" t="s">
+        <v>62</v>
+      </c>
+      <c r="B642" s="1">
+        <v>45685.456944444442</v>
+      </c>
+      <c r="C642" s="2">
+        <v>1.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upated all old Superstition hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="104">
   <si>
     <t>DateTime</t>
   </si>
@@ -655,12 +655,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E663"/>
+  <dimension ref="A1:E666"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A647" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="E664" sqref="E664"/>
+      <selection pane="bottomLeft" activeCell="C665" sqref="C665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9331,6 +9331,42 @@
         <v>91</v>
       </c>
     </row>
+    <row r="664" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A664" t="s">
+        <v>62</v>
+      </c>
+      <c r="B664" s="1">
+        <v>45707.5</v>
+      </c>
+      <c r="C664">
+        <v>1.87</v>
+      </c>
+      <c r="E664" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A665" t="s">
+        <v>62</v>
+      </c>
+      <c r="B665" s="1">
+        <v>45708.548611111109</v>
+      </c>
+      <c r="C665">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="666" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A666" t="s">
+        <v>62</v>
+      </c>
+      <c r="B666" s="1">
+        <v>45709.46875</v>
+      </c>
+      <c r="C666">
+        <v>1.87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Picacho Peak NM
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="104">
   <si>
     <t>DateTime</t>
   </si>
@@ -655,12 +655,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E667"/>
+  <dimension ref="A1:E668"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A652" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A667" sqref="A667"/>
+      <selection pane="bottomLeft" activeCell="D668" sqref="D668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9384,6 +9384,17 @@
         <v>91</v>
       </c>
     </row>
+    <row r="668" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A668" t="s">
+        <v>62</v>
+      </c>
+      <c r="B668" s="1">
+        <v>45711.642361111109</v>
+      </c>
+      <c r="C668">
+        <v>1.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Va Beach hikes, plus some other updates
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="106">
   <si>
     <t>DateTime</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Lots of snow melt started here</t>
+  </si>
+  <si>
+    <t>Rain, not SWE (but still ice on lakes)</t>
   </si>
 </sst>
 </file>
@@ -658,17 +661,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E676"/>
+  <dimension ref="A1:E687"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A654" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A669" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A671" sqref="A671:A676"/>
+      <selection pane="bottomLeft" activeCell="E683" sqref="E683"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="5" max="5" width="54.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -684,7 +688,7 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
@@ -701,7 +705,7 @@
       <c r="B5" s="1">
         <v>45048.45208333333</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2.34</v>
       </c>
       <c r="D5">
@@ -718,7 +722,7 @@
       <c r="B6" s="1">
         <v>45049.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>2.33</v>
       </c>
       <c r="E6" t="s">
@@ -732,7 +736,7 @@
       <c r="B7" s="1">
         <v>45050.508333333331</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>2.3199999999999998</v>
       </c>
       <c r="E7" t="s">
@@ -746,7 +750,7 @@
       <c r="B8" s="1">
         <v>45051.636111111111</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>2.2799999999999998</v>
       </c>
     </row>
@@ -757,7 +761,7 @@
       <c r="B9" s="1">
         <v>45052.484722222223</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>2.27</v>
       </c>
     </row>
@@ -768,7 +772,7 @@
       <c r="B10" s="1">
         <v>45053.447916666664</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>2.2799999999999998</v>
       </c>
       <c r="D10">
@@ -785,7 +789,7 @@
       <c r="B11" s="1">
         <v>45054.690972222219</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>2.2599999999999998</v>
       </c>
     </row>
@@ -796,7 +800,7 @@
       <c r="B12" s="1">
         <v>45055.57708333333</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>2.29</v>
       </c>
       <c r="D12">
@@ -813,7 +817,7 @@
       <c r="B13" s="1">
         <v>45056.46597222222</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>2.29</v>
       </c>
       <c r="D13">
@@ -830,7 +834,7 @@
       <c r="B14" s="1">
         <v>45057.388194444444</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>2.2599999999999998</v>
       </c>
     </row>
@@ -841,7 +845,7 @@
       <c r="B15" s="1">
         <v>45058.433333333334</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>2.2400000000000002</v>
       </c>
       <c r="E15" t="s">
@@ -855,7 +859,7 @@
       <c r="B16" s="1">
         <v>45059.370833333334</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -866,7 +870,7 @@
       <c r="B17" s="1">
         <v>45060.85833333333</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>2.17</v>
       </c>
     </row>
@@ -7572,7 +7576,7 @@
       <c r="B534" s="1">
         <v>45577.456250000003</v>
       </c>
-      <c r="C534">
+      <c r="C534" s="2">
         <v>1.69</v>
       </c>
       <c r="E534" t="s">
@@ -7586,7 +7590,7 @@
       <c r="B535" s="1">
         <v>45578.491666666669</v>
       </c>
-      <c r="C535">
+      <c r="C535" s="2">
         <v>1.71</v>
       </c>
       <c r="D535">
@@ -7787,7 +7791,7 @@
       <c r="B550" s="1">
         <v>45593.5</v>
       </c>
-      <c r="C550">
+      <c r="C550" s="2">
         <v>1.81</v>
       </c>
       <c r="E550" t="s">
@@ -7801,7 +7805,7 @@
       <c r="B551" s="1">
         <v>45594.535416666666</v>
       </c>
-      <c r="C551">
+      <c r="C551" s="2">
         <v>1.81</v>
       </c>
       <c r="E551" t="s">
@@ -8808,7 +8812,7 @@
       <c r="B627" s="1">
         <v>45670.541666666664</v>
       </c>
-      <c r="C627">
+      <c r="C627" s="2">
         <v>1.88</v>
       </c>
       <c r="D627">
@@ -9068,7 +9072,7 @@
       <c r="B646" s="1">
         <v>45689.493750000001</v>
       </c>
-      <c r="C646">
+      <c r="C646" s="2">
         <v>1.84</v>
       </c>
       <c r="E646" t="s">
@@ -9099,7 +9103,7 @@
       <c r="B648" s="1">
         <v>45691.523611111108</v>
       </c>
-      <c r="C648">
+      <c r="C648" s="2">
         <v>1.85</v>
       </c>
     </row>
@@ -9127,7 +9131,7 @@
       <c r="B650" s="1">
         <v>45693.5625</v>
       </c>
-      <c r="C650">
+      <c r="C650" s="2">
         <v>1.85</v>
       </c>
     </row>
@@ -9155,7 +9159,7 @@
       <c r="B652" s="1">
         <v>45695.5</v>
       </c>
-      <c r="C652">
+      <c r="C652" s="2">
         <v>1.88</v>
       </c>
       <c r="E652" t="s">
@@ -9169,7 +9173,7 @@
       <c r="B653" s="1">
         <v>45696.5</v>
       </c>
-      <c r="C653">
+      <c r="C653" s="2">
         <v>1.88</v>
       </c>
       <c r="D653">
@@ -9186,7 +9190,7 @@
       <c r="B654" s="1">
         <v>45697.5</v>
       </c>
-      <c r="C654">
+      <c r="C654" s="2">
         <v>1.88</v>
       </c>
       <c r="D654">
@@ -9203,7 +9207,7 @@
       <c r="B655" s="1">
         <v>45698.5</v>
       </c>
-      <c r="C655">
+      <c r="C655" s="2">
         <v>1.88</v>
       </c>
       <c r="E655" t="s">
@@ -9217,7 +9221,7 @@
       <c r="B656" s="1">
         <v>45699.5</v>
       </c>
-      <c r="C656">
+      <c r="C656" s="2">
         <v>1.86</v>
       </c>
       <c r="E656" t="s">
@@ -9231,7 +9235,7 @@
       <c r="B657" s="1">
         <v>45700.5</v>
       </c>
-      <c r="C657">
+      <c r="C657" s="2">
         <v>1.84</v>
       </c>
       <c r="E657" t="s">
@@ -9245,7 +9249,7 @@
       <c r="B658" s="1">
         <v>45701.5</v>
       </c>
-      <c r="C658">
+      <c r="C658" s="2">
         <v>1.84</v>
       </c>
       <c r="E658" t="s">
@@ -9259,7 +9263,7 @@
       <c r="B659" s="1">
         <v>45702.5</v>
       </c>
-      <c r="C659">
+      <c r="C659" s="2">
         <v>1.84</v>
       </c>
       <c r="E659" t="s">
@@ -9273,7 +9277,7 @@
       <c r="B660" s="1">
         <v>45703.5</v>
       </c>
-      <c r="C660">
+      <c r="C660" s="2">
         <v>1.87</v>
       </c>
       <c r="D660">
@@ -9290,7 +9294,7 @@
       <c r="B661" s="1">
         <v>45704.5</v>
       </c>
-      <c r="C661">
+      <c r="C661" s="2">
         <v>1.87</v>
       </c>
       <c r="D661">
@@ -9307,7 +9311,7 @@
       <c r="B662" s="1">
         <v>45705.5</v>
       </c>
-      <c r="C662">
+      <c r="C662" s="2">
         <v>1.87</v>
       </c>
       <c r="D662">
@@ -9324,7 +9328,7 @@
       <c r="B663" s="1">
         <v>45706.5625</v>
       </c>
-      <c r="C663">
+      <c r="C663" s="2">
         <v>1.87</v>
       </c>
       <c r="D663">
@@ -9341,7 +9345,7 @@
       <c r="B664" s="1">
         <v>45707.5</v>
       </c>
-      <c r="C664">
+      <c r="C664" s="2">
         <v>1.87</v>
       </c>
       <c r="E664" t="s">
@@ -9355,7 +9359,7 @@
       <c r="B665" s="1">
         <v>45708.548611111109</v>
       </c>
-      <c r="C665">
+      <c r="C665" s="2">
         <v>1.86</v>
       </c>
     </row>
@@ -9366,7 +9370,7 @@
       <c r="B666" s="1">
         <v>45709.46875</v>
       </c>
-      <c r="C666">
+      <c r="C666" s="2">
         <v>1.87</v>
       </c>
     </row>
@@ -9377,7 +9381,7 @@
       <c r="B667" s="1">
         <v>45710.456250000003</v>
       </c>
-      <c r="C667">
+      <c r="C667" s="2">
         <v>1.86</v>
       </c>
       <c r="D667">
@@ -9394,7 +9398,7 @@
       <c r="B668" s="1">
         <v>45711.642361111109</v>
       </c>
-      <c r="C668">
+      <c r="C668" s="2">
         <v>1.85</v>
       </c>
     </row>
@@ -9405,7 +9409,7 @@
       <c r="B669" s="1">
         <v>45712.626388888886</v>
       </c>
-      <c r="C669">
+      <c r="C669" s="2">
         <v>1.86</v>
       </c>
       <c r="E669" t="s">
@@ -9419,7 +9423,7 @@
       <c r="B670" s="1">
         <v>45713.506249999999</v>
       </c>
-      <c r="C670">
+      <c r="C670" s="2">
         <v>1.86</v>
       </c>
     </row>
@@ -9430,7 +9434,7 @@
       <c r="B671" s="1">
         <v>45714.5</v>
       </c>
-      <c r="C671">
+      <c r="C671" s="2">
         <v>1.86</v>
       </c>
       <c r="E671" t="s">
@@ -9444,7 +9448,7 @@
       <c r="B672" s="1">
         <v>45715.5</v>
       </c>
-      <c r="C672">
+      <c r="C672" s="2">
         <v>1.86</v>
       </c>
       <c r="E672" t="s">
@@ -9458,7 +9462,7 @@
       <c r="B673" s="1">
         <v>45716.5</v>
       </c>
-      <c r="C673">
+      <c r="C673" s="2">
         <v>1.86</v>
       </c>
       <c r="E673" t="s">
@@ -9472,7 +9476,7 @@
       <c r="B674" s="1">
         <v>45717.5</v>
       </c>
-      <c r="C674">
+      <c r="C674" s="2">
         <v>1.86</v>
       </c>
       <c r="E674" t="s">
@@ -9486,7 +9490,7 @@
       <c r="B675" s="1">
         <v>45718.5</v>
       </c>
-      <c r="C675">
+      <c r="C675" s="2">
         <v>1.86</v>
       </c>
       <c r="E675" t="s">
@@ -9500,8 +9504,147 @@
       <c r="B676" s="1">
         <v>45719.583333333336</v>
       </c>
-      <c r="C676">
+      <c r="C676" s="2">
         <v>1.86</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A677" t="s">
+        <v>62</v>
+      </c>
+      <c r="B677" s="1">
+        <v>45720.520833333336</v>
+      </c>
+      <c r="C677" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="D677">
+        <v>0.3</v>
+      </c>
+      <c r="E677" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="678" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A678" t="s">
+        <v>62</v>
+      </c>
+      <c r="B678" s="1">
+        <v>45356.690972222219</v>
+      </c>
+      <c r="C678" s="2">
+        <v>1.93</v>
+      </c>
+      <c r="D678">
+        <v>0.35</v>
+      </c>
+      <c r="E678" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="679" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A679" t="s">
+        <v>62</v>
+      </c>
+      <c r="B679" s="1">
+        <v>45722.504861111112</v>
+      </c>
+      <c r="C679" s="2">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="680" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A680" t="s">
+        <v>62</v>
+      </c>
+      <c r="B680" s="1">
+        <v>45723.525694444441</v>
+      </c>
+      <c r="C680" s="2">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="681" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A681" t="s">
+        <v>62</v>
+      </c>
+      <c r="B681" s="1">
+        <v>45724.487500000003</v>
+      </c>
+      <c r="C681" s="2">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="682" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A682" t="s">
+        <v>62</v>
+      </c>
+      <c r="B682" s="1">
+        <v>45725.5</v>
+      </c>
+      <c r="C682" s="2">
+        <v>1.91</v>
+      </c>
+      <c r="E682" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="683" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A683" t="s">
+        <v>62</v>
+      </c>
+      <c r="B683" s="1">
+        <v>45726.556944444441</v>
+      </c>
+      <c r="C683" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="E683" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="684" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A684" t="s">
+        <v>62</v>
+      </c>
+      <c r="B684" s="1">
+        <v>45727.542361111111</v>
+      </c>
+      <c r="C684" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="685" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A685" t="s">
+        <v>62</v>
+      </c>
+      <c r="B685" s="1">
+        <v>45728.565972222219</v>
+      </c>
+      <c r="C685" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="686" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A686" t="s">
+        <v>62</v>
+      </c>
+      <c r="B686" s="1">
+        <v>45729.698611111111</v>
+      </c>
+      <c r="C686" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="687" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A687" t="s">
+        <v>62</v>
+      </c>
+      <c r="B687" s="1">
+        <v>45730.643750000003</v>
+      </c>
+      <c r="C687" s="2">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Tucson hikes to Other, re-rendered
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="106">
   <si>
     <t>DateTime</t>
   </si>
@@ -661,12 +661,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E688"/>
+  <dimension ref="A1:E690"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A671" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A672" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
+      <selection pane="bottomLeft" activeCell="A689" sqref="A689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9664,6 +9664,19 @@
         <v>105</v>
       </c>
     </row>
+    <row r="689" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A689" t="s">
+        <v>62</v>
+      </c>
+      <c r="E689" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="690" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A690" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Pinicon Ridge and Osborne Park
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="107">
   <si>
     <t>DateTime</t>
   </si>
@@ -664,12 +664,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E705"/>
+  <dimension ref="A1:E706"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A705" sqref="A705"/>
+      <selection pane="bottomLeft" activeCell="A706" sqref="A706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9879,7 +9879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="705" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="705" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A705" t="s">
         <v>62</v>
       </c>
@@ -9888,6 +9888,23 @@
       </c>
       <c r="C705" s="2">
         <v>1.94</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A706" t="s">
+        <v>62</v>
+      </c>
+      <c r="B706" s="1">
+        <v>45749.527777777781</v>
+      </c>
+      <c r="C706" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="D706">
+        <v>0.15</v>
+      </c>
+      <c r="E706" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to some portfolio posts
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="107">
   <si>
     <t>DateTime</t>
   </si>
@@ -664,7 +664,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E708"/>
+  <dimension ref="A1:E709"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
@@ -9935,6 +9935,23 @@
         <v>1.98</v>
       </c>
     </row>
+    <row r="709" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A709" t="s">
+        <v>62</v>
+      </c>
+      <c r="B709" s="1">
+        <v>45752.534722222219</v>
+      </c>
+      <c r="C709" s="2">
+        <v>2</v>
+      </c>
+      <c r="D709">
+        <v>0.04</v>
+      </c>
+      <c r="E709" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added recent DLH hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="106">
   <si>
     <t>DateTime</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Cleaned grate before reading</t>
   </si>
   <si>
-    <t>Extrapolated</t>
-  </si>
-  <si>
     <t>Snowing at observation time</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>Kevin did reading</t>
   </si>
   <si>
-    <t>SWE; Extrapolated</t>
-  </si>
-  <si>
     <t>SWE; Kevin did reading</t>
   </si>
   <si>
@@ -345,6 +339,9 @@
   </si>
   <si>
     <t>Joseph took measurements</t>
+  </si>
+  <si>
+    <t>SWE; Interpolated</t>
   </si>
 </sst>
 </file>
@@ -664,12 +661,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E709"/>
+  <dimension ref="A1:E712"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A708" sqref="A708"/>
+      <selection pane="bottomLeft" activeCell="A710" sqref="A710:A712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7770,7 +7767,7 @@
         <v>1.82</v>
       </c>
       <c r="E548" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.3">
@@ -7784,7 +7781,7 @@
         <v>1.82</v>
       </c>
       <c r="E549" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.3">
@@ -7798,7 +7795,7 @@
         <v>1.81</v>
       </c>
       <c r="E550" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.3">
@@ -7843,7 +7840,7 @@
         <v>0.48</v>
       </c>
       <c r="E553" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.3">
@@ -7902,7 +7899,7 @@
         <v>0.52</v>
       </c>
       <c r="E557" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.3">
@@ -7980,7 +7977,7 @@
         <v>0.15</v>
       </c>
       <c r="E563" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.3">
@@ -7994,7 +7991,7 @@
         <v>1.98</v>
       </c>
       <c r="E564" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.3">
@@ -8008,7 +8005,7 @@
         <v>1.9</v>
       </c>
       <c r="E565" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.3">
@@ -8166,7 +8163,7 @@
         <v>0.25</v>
       </c>
       <c r="E578" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.3">
@@ -8180,7 +8177,7 @@
         <v>1.92</v>
       </c>
       <c r="E579" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.3">
@@ -8194,7 +8191,7 @@
         <v>1.91</v>
       </c>
       <c r="E580" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.3">
@@ -8208,7 +8205,7 @@
         <v>1.9</v>
       </c>
       <c r="E581" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.3">
@@ -8225,7 +8222,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E582" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.3">
@@ -8242,7 +8239,7 @@
         <v>0.06</v>
       </c>
       <c r="E583" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.3">
@@ -8259,7 +8256,7 @@
         <v>0.02</v>
       </c>
       <c r="E584" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.3">
@@ -8298,7 +8295,7 @@
         <v>0.1</v>
       </c>
       <c r="E587" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.3">
@@ -8315,7 +8312,7 @@
         <v>0.1</v>
       </c>
       <c r="E588" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.3">
@@ -8365,7 +8362,7 @@
         <v>0.31</v>
       </c>
       <c r="E592" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.3">
@@ -8382,7 +8379,7 @@
         <v>0.01</v>
       </c>
       <c r="E593" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.3">
@@ -8399,7 +8396,7 @@
         <v>0.04</v>
       </c>
       <c r="E594" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.3">
@@ -8416,7 +8413,7 @@
         <v>0.04</v>
       </c>
       <c r="E595" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.3">
@@ -8430,7 +8427,7 @@
         <v>1.89</v>
       </c>
       <c r="E596" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.3">
@@ -8480,7 +8477,7 @@
         <v>0.01</v>
       </c>
       <c r="E600" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.3">
@@ -8497,7 +8494,7 @@
         <v>0.01</v>
       </c>
       <c r="E601" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.3">
@@ -8525,7 +8522,7 @@
         <v>0.13</v>
       </c>
       <c r="E603" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.3">
@@ -8605,7 +8602,7 @@
         <v>1.86</v>
       </c>
       <c r="E610" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.3">
@@ -8622,7 +8619,7 @@
         <v>0.53</v>
       </c>
       <c r="E611" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.3">
@@ -8672,7 +8669,7 @@
         <v>0.01</v>
       </c>
       <c r="E615" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.3">
@@ -8788,7 +8785,7 @@
         <v>1.87</v>
       </c>
       <c r="E625" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.3">
@@ -8805,7 +8802,7 @@
         <v>0.22</v>
       </c>
       <c r="E626" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.3">
@@ -8822,7 +8819,7 @@
         <v>0.15</v>
       </c>
       <c r="E627" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.3">
@@ -8839,7 +8836,7 @@
         <v>0.01</v>
       </c>
       <c r="E628" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.3">
@@ -8853,7 +8850,7 @@
         <v>1.86</v>
       </c>
       <c r="E629" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.3">
@@ -8870,7 +8867,7 @@
         <v>0.03</v>
       </c>
       <c r="E630" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.3">
@@ -8909,7 +8906,7 @@
         <v>0.01</v>
       </c>
       <c r="E633" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.3">
@@ -8923,7 +8920,7 @@
         <v>1.86</v>
       </c>
       <c r="E634" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.3">
@@ -8940,7 +8937,7 @@
         <v>0.06</v>
       </c>
       <c r="E635" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.3">
@@ -8957,7 +8954,7 @@
         <v>0.03</v>
       </c>
       <c r="E636" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.3">
@@ -9015,7 +9012,7 @@
         <v>1.86</v>
       </c>
       <c r="E641" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="642" spans="1:5" x14ac:dyDescent="0.3">
@@ -9040,7 +9037,7 @@
         <v>1.86</v>
       </c>
       <c r="E643" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="644" spans="1:5" x14ac:dyDescent="0.3">
@@ -9065,7 +9062,7 @@
         <v>1.85</v>
       </c>
       <c r="E645" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.3">
@@ -9079,7 +9076,7 @@
         <v>1.84</v>
       </c>
       <c r="E646" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="647" spans="1:5" x14ac:dyDescent="0.3">
@@ -9096,7 +9093,7 @@
         <v>0.16</v>
       </c>
       <c r="E647" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="648" spans="1:5" x14ac:dyDescent="0.3">
@@ -9124,7 +9121,7 @@
         <v>0.01</v>
       </c>
       <c r="E649" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.3">
@@ -9152,7 +9149,7 @@
         <v>0.26</v>
       </c>
       <c r="E651" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.3">
@@ -9166,7 +9163,7 @@
         <v>1.88</v>
       </c>
       <c r="E652" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.3">
@@ -9183,7 +9180,7 @@
         <v>0.15</v>
       </c>
       <c r="E653" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="654" spans="1:5" x14ac:dyDescent="0.3">
@@ -9200,7 +9197,7 @@
         <v>0.05</v>
       </c>
       <c r="E654" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.3">
@@ -9214,7 +9211,7 @@
         <v>1.88</v>
       </c>
       <c r="E655" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.3">
@@ -9228,7 +9225,7 @@
         <v>1.86</v>
       </c>
       <c r="E656" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="657" spans="1:5" x14ac:dyDescent="0.3">
@@ -9242,7 +9239,7 @@
         <v>1.84</v>
       </c>
       <c r="E657" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="658" spans="1:5" x14ac:dyDescent="0.3">
@@ -9256,7 +9253,7 @@
         <v>1.84</v>
       </c>
       <c r="E658" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.3">
@@ -9270,7 +9267,7 @@
         <v>1.84</v>
       </c>
       <c r="E659" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.3">
@@ -9287,7 +9284,7 @@
         <v>0.17</v>
       </c>
       <c r="E660" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.3">
@@ -9304,7 +9301,7 @@
         <v>0.05</v>
       </c>
       <c r="E661" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.3">
@@ -9321,7 +9318,7 @@
         <v>0.02</v>
       </c>
       <c r="E662" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.3">
@@ -9338,7 +9335,7 @@
         <v>0.01</v>
       </c>
       <c r="E663" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.3">
@@ -9352,7 +9349,7 @@
         <v>1.87</v>
       </c>
       <c r="E664" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.3">
@@ -9391,7 +9388,7 @@
         <v>0.02</v>
       </c>
       <c r="E667" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="668" spans="1:5" x14ac:dyDescent="0.3">
@@ -9416,7 +9413,7 @@
         <v>1.86</v>
       </c>
       <c r="E669" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.3">
@@ -9441,7 +9438,7 @@
         <v>1.86</v>
       </c>
       <c r="E671" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="672" spans="1:5" x14ac:dyDescent="0.3">
@@ -9455,7 +9452,7 @@
         <v>1.86</v>
       </c>
       <c r="E672" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.3">
@@ -9469,7 +9466,7 @@
         <v>1.86</v>
       </c>
       <c r="E673" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.3">
@@ -9483,7 +9480,7 @@
         <v>1.86</v>
       </c>
       <c r="E674" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="675" spans="1:5" x14ac:dyDescent="0.3">
@@ -9497,7 +9494,7 @@
         <v>1.86</v>
       </c>
       <c r="E675" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="676" spans="1:5" x14ac:dyDescent="0.3">
@@ -9525,7 +9522,7 @@
         <v>0.3</v>
       </c>
       <c r="E677" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.3">
@@ -9542,7 +9539,7 @@
         <v>0.35</v>
       </c>
       <c r="E678" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.3">
@@ -9589,7 +9586,7 @@
         <v>1.91</v>
       </c>
       <c r="E682" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="683" spans="1:5" x14ac:dyDescent="0.3">
@@ -9603,7 +9600,7 @@
         <v>1.9</v>
       </c>
       <c r="E683" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="684" spans="1:5" x14ac:dyDescent="0.3">
@@ -9664,7 +9661,7 @@
         <v>0.05</v>
       </c>
       <c r="E688" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.3">
@@ -9678,7 +9675,7 @@
         <v>1.9</v>
       </c>
       <c r="E689" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.3">
@@ -9775,7 +9772,7 @@
         <v>0.19</v>
       </c>
       <c r="E697" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.3">
@@ -9789,7 +9786,7 @@
         <v>1.92</v>
       </c>
       <c r="E698" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="699" spans="1:5" x14ac:dyDescent="0.3">
@@ -9803,7 +9800,7 @@
         <v>1.92</v>
       </c>
       <c r="E699" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.3">
@@ -9817,7 +9814,7 @@
         <v>1.9</v>
       </c>
       <c r="E700" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="701" spans="1:5" x14ac:dyDescent="0.3">
@@ -9862,7 +9859,7 @@
         <v>0.49</v>
       </c>
       <c r="E703" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="704" spans="1:5" x14ac:dyDescent="0.3">
@@ -9876,7 +9873,7 @@
         <v>1.96</v>
       </c>
       <c r="E704" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="705" spans="1:5" x14ac:dyDescent="0.3">
@@ -9904,7 +9901,7 @@
         <v>0.15</v>
       </c>
       <c r="E706" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="707" spans="1:5" x14ac:dyDescent="0.3">
@@ -9921,7 +9918,7 @@
         <v>0.37</v>
       </c>
       <c r="E707" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="708" spans="1:5" x14ac:dyDescent="0.3">
@@ -9949,7 +9946,43 @@
         <v>0.04</v>
       </c>
       <c r="E709" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A710" t="s">
+        <v>62</v>
+      </c>
+      <c r="B710" s="1">
+        <v>45753.600694444445</v>
+      </c>
+      <c r="C710" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A711" t="s">
+        <v>62</v>
+      </c>
+      <c r="B711" s="1">
+        <v>45754.5</v>
+      </c>
+      <c r="C711" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="E711" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A712" t="s">
+        <v>62</v>
+      </c>
+      <c r="B712" s="1">
+        <v>45755.506249999999</v>
+      </c>
+      <c r="C712" s="2">
+        <v>1.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Dam Readings Page
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="109">
   <si>
     <t>DateTime</t>
   </si>
@@ -342,6 +342,15 @@
   </si>
   <si>
     <t>SWE; Interpolated</t>
+  </si>
+  <si>
+    <t>Rain (not SWE)</t>
+  </si>
+  <si>
+    <t>Mixed (so SWE); Official Eagle lake ice out</t>
+  </si>
+  <si>
+    <t>2025-26</t>
   </si>
 </sst>
 </file>
@@ -661,12 +670,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E712"/>
+  <dimension ref="A1:E720"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A693" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A710" sqref="A710:A712"/>
+      <selection pane="bottomLeft" activeCell="A720" sqref="A720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9084,7 +9093,7 @@
         <v>62</v>
       </c>
       <c r="B647" s="1">
-        <v>45324.5</v>
+        <v>45690.5</v>
       </c>
       <c r="C647" s="2">
         <v>1.86</v>
@@ -9530,7 +9539,7 @@
         <v>62</v>
       </c>
       <c r="B678" s="1">
-        <v>45356.690972222219</v>
+        <v>45721.690972222219</v>
       </c>
       <c r="C678" s="2">
         <v>1.93</v>
@@ -9983,6 +9992,127 @@
       </c>
       <c r="C712" s="2">
         <v>1.96</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A713" t="s">
+        <v>62</v>
+      </c>
+      <c r="B713" s="1">
+        <v>45756.449305555558</v>
+      </c>
+      <c r="C713" s="2">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A714" t="s">
+        <v>62</v>
+      </c>
+      <c r="B714" s="1">
+        <v>45757.505555555559</v>
+      </c>
+      <c r="C714" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="D714">
+        <v>0.03</v>
+      </c>
+      <c r="E714" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A715" t="s">
+        <v>62</v>
+      </c>
+      <c r="B715" s="1">
+        <v>45758.6875</v>
+      </c>
+      <c r="C715" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="D715">
+        <v>0.01</v>
+      </c>
+      <c r="E715" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A716" t="s">
+        <v>62</v>
+      </c>
+      <c r="B716" s="1">
+        <v>45759.540277777778</v>
+      </c>
+      <c r="C716" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="E716" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A717" t="s">
+        <v>62</v>
+      </c>
+      <c r="B717" s="1">
+        <v>45760.499305555553</v>
+      </c>
+      <c r="C717" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="D717">
+        <v>0.08</v>
+      </c>
+      <c r="E717" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A718" t="s">
+        <v>62</v>
+      </c>
+      <c r="B718" s="1">
+        <v>45761.541666666664</v>
+      </c>
+      <c r="C718" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="D718">
+        <v>0.09</v>
+      </c>
+      <c r="E718" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A719" t="s">
+        <v>108</v>
+      </c>
+      <c r="B719" s="1">
+        <v>45762.522222222222</v>
+      </c>
+      <c r="C719" s="2">
+        <v>2</v>
+      </c>
+      <c r="D719">
+        <v>0.37</v>
+      </c>
+      <c r="E719" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A720" t="s">
+        <v>108</v>
+      </c>
+      <c r="B720" s="1">
+        <v>45763.513194444444</v>
+      </c>
+      <c r="C720" s="2">
+        <v>1.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two WI hikes
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="131">
   <si>
     <t>DateTime</t>
   </si>
@@ -740,12 +740,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E985"/>
+  <dimension ref="A1:E997"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A966" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A978" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A985" sqref="A985"/>
+      <selection pane="bottomLeft" activeCell="D998" sqref="D998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13637,6 +13637,186 @@
         <v>1.83</v>
       </c>
     </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A986" t="s">
+        <v>108</v>
+      </c>
+      <c r="B986" s="1">
+        <v>46029.5</v>
+      </c>
+      <c r="C986" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="E986" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="987" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A987" t="s">
+        <v>108</v>
+      </c>
+      <c r="B987" s="1">
+        <v>46030.384722222225</v>
+      </c>
+      <c r="C987" s="2">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="988" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A988" t="s">
+        <v>108</v>
+      </c>
+      <c r="B988" s="1">
+        <v>46031.466666666667</v>
+      </c>
+      <c r="C988" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="989" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A989" t="s">
+        <v>108</v>
+      </c>
+      <c r="B989" s="1">
+        <v>46032.5</v>
+      </c>
+      <c r="C989" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D989">
+        <v>0.03</v>
+      </c>
+      <c r="E989" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="990" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A990" t="s">
+        <v>108</v>
+      </c>
+      <c r="B990" s="1">
+        <v>46033.520833333336</v>
+      </c>
+      <c r="C990" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D990">
+        <v>0.04</v>
+      </c>
+      <c r="E990" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="991" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A991" t="s">
+        <v>108</v>
+      </c>
+      <c r="B991" s="1">
+        <v>46034.534722222219</v>
+      </c>
+      <c r="C991" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="992" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A992" t="s">
+        <v>108</v>
+      </c>
+      <c r="B992" s="1">
+        <v>46035.498611111114</v>
+      </c>
+      <c r="C992" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D992">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E992" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="993" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A993" t="s">
+        <v>108</v>
+      </c>
+      <c r="B993" s="1">
+        <v>46036.520833333336</v>
+      </c>
+      <c r="C993" s="2">
+        <v>1.84</v>
+      </c>
+      <c r="D993">
+        <v>0.01</v>
+      </c>
+      <c r="E993" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="994" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A994" t="s">
+        <v>108</v>
+      </c>
+      <c r="B994" s="1">
+        <v>46037.5</v>
+      </c>
+      <c r="C994" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="E994" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="995" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A995" t="s">
+        <v>108</v>
+      </c>
+      <c r="B995" s="1">
+        <v>46038.583333333336</v>
+      </c>
+      <c r="C995" s="2">
+        <v>1.86</v>
+      </c>
+      <c r="D995">
+        <v>0.4</v>
+      </c>
+      <c r="E995" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="996" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A996" t="s">
+        <v>108</v>
+      </c>
+      <c r="B996" s="1">
+        <v>46039.594444444447</v>
+      </c>
+      <c r="C996" s="2">
+        <v>1.84</v>
+      </c>
+      <c r="D996">
+        <v>0.04</v>
+      </c>
+      <c r="E996" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="997" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A997" t="s">
+        <v>108</v>
+      </c>
+      <c r="B997" s="1">
+        <v>46040.602777777778</v>
+      </c>
+      <c r="C997" s="2">
+        <v>1.86</v>
+      </c>
+      <c r="D997">
+        <v>0.01</v>
+      </c>
+      <c r="E997" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Linville Gorge Hike
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="131">
   <si>
     <t>DateTime</t>
   </si>
@@ -740,12 +740,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E997"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A978" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D998" sqref="D998"/>
+      <selection pane="bottomLeft" activeCell="A1000" sqref="A1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13817,6 +13817,54 @@
         <v>90</v>
       </c>
     </row>
+    <row r="998" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A998" t="s">
+        <v>108</v>
+      </c>
+      <c r="B998" s="1">
+        <v>46041.5</v>
+      </c>
+      <c r="C998" s="2">
+        <v>1.86</v>
+      </c>
+      <c r="D998">
+        <v>0.12</v>
+      </c>
+      <c r="E998" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="999" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A999" t="s">
+        <v>108</v>
+      </c>
+      <c r="B999" s="1">
+        <v>46042.5</v>
+      </c>
+      <c r="C999" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="E999" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1000" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1000" s="1">
+        <v>46043.572916666664</v>
+      </c>
+      <c r="C1000" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="D1000">
+        <v>0.01</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added several IR tracks to mapping
</commit_message>
<xml_diff>
--- a/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
+++ b/portfolio/posts/_data/Flynn_Dam_Heights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="131">
   <si>
     <t>DateTime</t>
   </si>
@@ -740,12 +740,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1004"/>
+  <dimension ref="A1:E1016"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A978" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A999" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A1004" sqref="A1004"/>
+      <selection pane="bottomLeft" activeCell="B1017" sqref="B1017"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13915,6 +13915,180 @@
         <v>1.83</v>
       </c>
     </row>
+    <row r="1005" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1005" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1005" s="1">
+        <v>46048.5</v>
+      </c>
+      <c r="C1005" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1006" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1006" s="1">
+        <v>46049.5625</v>
+      </c>
+      <c r="C1006" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1007" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1007" s="1">
+        <v>46050.5</v>
+      </c>
+      <c r="C1007" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="D1007">
+        <v>0.02</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1008" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1008" s="1">
+        <v>46051.552083333336</v>
+      </c>
+      <c r="C1008" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D1008">
+        <v>0.02</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1009" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1009" s="1">
+        <v>46052.5</v>
+      </c>
+      <c r="C1009" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D1009">
+        <v>0.03</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1010" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1010" s="1">
+        <v>46053.5</v>
+      </c>
+      <c r="C1010" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1011" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1011" s="1">
+        <v>46054.5</v>
+      </c>
+      <c r="C1011" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1012" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1012" s="1">
+        <v>46055.565972222219</v>
+      </c>
+      <c r="C1012" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="D1012">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1013" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1013" s="1">
+        <v>46056.5</v>
+      </c>
+      <c r="C1013" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1014" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1014" s="1">
+        <v>46057.5</v>
+      </c>
+      <c r="C1014" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1015" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1015" s="1">
+        <v>46058.525694444441</v>
+      </c>
+      <c r="C1015" s="2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1016" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1016" s="1">
+        <v>46059.46875</v>
+      </c>
+      <c r="C1016" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="D1016">
+        <v>0.1</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>